<commit_message>
Added unbalanced images to simon-5501-12-slides
</commit_message>
<xml_diff>
--- a/biostats-1/12/data/unbalanced.xlsx
+++ b/biostats-1/12/data/unbalanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\git\classes\biostats-1\12\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\classes\biostats-1\12\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878AE4C0-F04D-4C97-86CC-B019977A38B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FAA030-D74F-476E-8735-7277E5BC7619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{8528FCC7-96F2-4FDC-B94D-642B522E5213}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8528FCC7-96F2-4FDC-B94D-642B522E5213}"/>
   </bookViews>
   <sheets>
     <sheet name="unbalanced" sheetId="1" r:id="rId1"/>
@@ -612,136 +612,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581270</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>96160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>224910</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104080</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2618350" y="644800"/>
-            <a:ext cx="964440" cy="7920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>613110</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>119350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>237310</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85150</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2650190" y="667990"/>
-            <a:ext cx="945000" cy="148680"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>7320</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -755,7 +625,7 @@
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
               <a:extLst>
@@ -943,8 +813,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="12" name="Ink 11">
@@ -963,7 +833,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="12" name="Ink 11">
@@ -985,916 +855,6 @@
             <a:xfrm>
               <a:off x="2894400" y="776160"/>
               <a:ext cx="12600" cy="12600"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>218560</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="13" name="Ink 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30AEC57C-4370-42DF-9931-EE6AB7F3F282}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2631440" y="1371600"/>
-            <a:ext cx="945000" cy="335280"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>589280</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>223640</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>86360</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="14" name="Ink 13">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65046459-87BD-4045-8DFD-E09486828D4F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2626360" y="1371600"/>
-            <a:ext cx="955160" cy="177800"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>599440</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>223640</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>92800</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="15" name="Ink 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18527F9F-8432-429E-82D8-5011C7CA4F46}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2636520" y="2504440"/>
-            <a:ext cx="945000" cy="148680"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>599440</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>223640</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="16" name="Ink 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CB196D6-382E-4583-A89E-E143185EA9D4}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2636520" y="3200400"/>
-            <a:ext cx="945000" cy="148680"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>591430</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>101240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>235070</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>109160</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="17" name="Ink 16">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5710972B-183B-49B4-BE91-26EB562692EC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2628510" y="2478680"/>
-            <a:ext cx="964440" cy="7920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>596510</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>80920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>240150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>88840</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="18" name="Ink 17">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69EDDBC1-A9CE-4ADB-85E9-76597EDC67BD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2633590" y="3189880"/>
-            <a:ext cx="964440" cy="7920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>111760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>227840</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>83923</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="21" name="Ink 20">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9B1B032-2337-4F34-ACE9-536D44D0CE93}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm flipV="1">
-            <a:off x="2616200" y="2306320"/>
-            <a:ext cx="969520" cy="155043"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>243080</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>48363</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="22" name="Ink 21">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E568CE5-77DD-4407-8F8D-39CE097D2C58}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm flipV="1">
-            <a:off x="2631440" y="3002280"/>
-            <a:ext cx="969520" cy="155043"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>217680</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>66246</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="23" name="Ink 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67337927-137C-40EE-B126-1E733363A804}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm flipV="1">
-            <a:off x="2621280" y="1193800"/>
-            <a:ext cx="954280" cy="152606"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>576190</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>80920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>219830</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>88840</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="24" name="Ink 23">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CCF8D95-8452-4891-8F9A-67FF623C631E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2613270" y="1361080"/>
-            <a:ext cx="964440" cy="7920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Ink 5">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB7707C-4C7B-D20B-6817-B49A733C3D07}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2271870" y="633600"/>
-              <a:ext cx="976680" cy="20160"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>492760</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>223520</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="25" name="Ink 24">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3CA43F5-2DA4-4347-93B1-2EF4C17AAF58}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3850640" y="1036320"/>
-            <a:ext cx="1102360" cy="335280"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>497840</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>208280</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="26" name="Ink 25">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9275CA4B-EB30-4654-9E4F-5EEF5A0FAFD0}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3855720" y="2824480"/>
-            <a:ext cx="1082040" cy="335280"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>116680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>203320</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>116840</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="27" name="Ink 26">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32D40584-391B-4420-A296-FD235B7167EB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm flipV="1">
-            <a:off x="3815080" y="665320"/>
-            <a:ext cx="1117720" cy="365920"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>96520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="28" name="Ink 27">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BF9AEEE-10B1-4733-9F56-0D1122BFD0CE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm flipV="1">
-            <a:off x="3840480" y="2473960"/>
-            <a:ext cx="1117720" cy="330200"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="8" name="Ink 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCAFC62-3A13-5113-B15D-4679294BE956}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2283390" y="656430"/>
-              <a:ext cx="957240" cy="160920"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2243,8 +1203,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="7" name="Ink 6">
@@ -2263,7 +1223,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="7" name="Ink 6">
@@ -3270,6 +2230,131 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>277800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>278160</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E75F3B7-E9F0-4563-937A-AD9D6B26A5A2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="887400" y="1531440"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389A55CB-E7CB-5B94-E316-59C53CBF9697}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="881280" y="1525320"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>277800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360" cy="360"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18A9CF4-72A0-4DB9-80BF-6F1B746CF6AA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="887400" y="1531440"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F967838A-B1CC-43DF-B3A4-F0DA0120DCE9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="881280" y="1525320"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3478,8 +2563,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="7" name="Ink 6">
@@ -3498,7 +2583,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="7" name="Ink 6">
@@ -4310,6 +3395,131 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>277800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>278160</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>68760</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D94CAD1-95E4-4B9C-83D2-4830B32B9F61}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="887400" y="1531440"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389A55CB-E7CB-5B94-E316-59C53CBF9697}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="881280" y="1525320"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>277800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>68400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="360" cy="360"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C525016-A0B3-4D82-974A-A311BD1EEB5B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="887400" y="1531440"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F967838A-B1CC-43DF-B3A4-F0DA0120DCE9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="881280" y="1525320"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4329,14 +3539,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:03:23.860"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:03:40.394"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4356,14 +3566,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:21:13.373"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.499"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 412 24307,'2624'-412'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4383,14 +3593,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:21:25.638"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.500"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 973 24307,'2527'-973'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4410,14 +3620,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:21:36.596"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.501"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 515 24307,'2556'-515'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4437,14 +3647,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:22:34.698"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.502"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2693'430'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 501 24307,'2584'-501'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4464,14 +3674,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:23:16.462"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.503"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2693'430'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 434 24307,'2584'-434'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4491,14 +3701,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:23:31.041"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.505"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2651'423'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 22 24379,'2581'-21'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4518,14 +3728,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:24:03.460"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.506"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2629'451'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4545,14 +3755,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:25:46.443"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.507"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'3061'-929'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2596'451'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4572,14 +3782,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:26:07.307"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.508"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'3005'-929'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2553'445'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4599,14 +3809,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:26:58.280"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.509"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3104'1014'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 22 24379,'2581'-21'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4626,14 +3836,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:03:35.647"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:04:27.322"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 412 24307,'2624'-412'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4653,18 +3863,747 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:27:32.109"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.510"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3104'915'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 973 24307,'2956'-973'0</inkml:trace>
 </inkml:ink>
 </file>
 
 <file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.511"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 973 24307,'2966'-973'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.512"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3042'1058'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.513"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3003'991'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:45:43.189"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 22 24379,'2581'-21'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:45:50.814"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 22 24379,'2581'-21'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink26.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T17:08:44.933"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink27.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T17:08:44.934"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink28.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.552"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink29.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.553"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:04:41.604"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink30.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.554"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink31.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.555"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink32.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.556"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1947 24307,'6323'-1947'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink33.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.557"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1462 24307,'6327'-1462'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink34.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.563"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6418'1488'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink35.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:34:23.444"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6161'1114'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink36.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:34:36.851"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6161'656'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink37.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:01.183"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6408'945'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink38.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:17.553"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6424'416'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink39.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:56.234"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 917 24307,'6316'-917'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:20:11.732"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink40.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:36:11.902"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 402 24307,'6316'-402'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink41.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:36:56.273"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 585 24307,'6316'-585'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink42.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:37:16.463"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1114 24307,'6316'-1114'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink43.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:37:36.075"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1573 24307,'6205'-1573'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink44.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T17:08:51.561"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink45.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T17:08:51.562"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4687,11 +4626,11 @@
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 22 24379,'2581'-21'0</inkml:trace>
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4714,11 +4653,11 @@
       <inkml:brushProperty name="height" value="0.035" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 458 24307,'2689'-458'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 479 24307,'2592'-479'0</inkml:trace>
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4745,7 +4684,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4772,7 +4711,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4796,1059 +4735,6 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink26.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.499"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink27.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.500"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'2624'-929'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink28.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.501"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 493 24307,'2652'-493'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink29.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.502"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 479 24307,'2680'-479'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:03:40.394"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink30.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.503"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 412 24307,'2680'-412'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink31.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.505"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink32.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.506"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2727'430'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink33.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.507"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2693'430'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink34.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.508"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'2651'423'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink35.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.509"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink36.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.510"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'3061'-929'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink37.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.511"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'3072'-929'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink38.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.512"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3147'1014'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink39.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:32.513"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2 24307,'3109'947'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:04:27.322"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink40.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:45:43.189"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink41.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:45:50.814"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 21 24379,'2677'-20'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink42.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.552"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink43.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.553"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink44.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.554"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink45.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.555"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink46.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.556"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1858 24307,'6524'-1858'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink47.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.557"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1395 24307,'6527'-1395'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink48.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:28:54.563"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6622'1423'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink49.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:34:23.444"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6364'1071'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T13:04:41.604"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink50.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:34:36.851"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6364'634'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink51.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:01.183"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6611'902'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink52.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:17.553"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 41 24379,'6627'394'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink53.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:35:56.234"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 873 24307,'6517'-873'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink54.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:36:11.902"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 380 24307,'6517'-380'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink55.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:36:56.273"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 563 24307,'6517'-563'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink56.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:37:16.463"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1070 24307,'6517'-1070'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink57.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:37:36.075"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1506 24307,'6406'-1506'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:20:11.732"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:20:21.213"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 929 24307,'2624'-929'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:20:37.268"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 493 24307,'2652'-493'0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-11T14:21:04.093"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 412 24307,'2624'-412'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -6169,23 +5055,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82076C0A-948B-4610-9B2E-7F2E55161CBB}">
-  <dimension ref="B2:H19"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6196,161 +5082,133 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <v>55</v>
       </c>
-      <c r="F4" s="1">
-        <f>AVERAGE(D4:D5)</f>
-        <v>50</v>
-      </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H6" s="1">
-        <f>AVERAGE(F4:F8)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>10</v>
       </c>
-      <c r="F8" s="1">
-        <f>AVERAGE(D7:D10)</f>
-        <v>20</v>
-      </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>45</v>
       </c>
-      <c r="F14" s="1">
-        <f>AVERAGE(D13:D15)</f>
-        <v>65</v>
-      </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H16" s="1">
-        <f>AVERAGE(F14:F18)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <v>85</v>
       </c>
-      <c r="F18" s="1">
-        <f>AVERAGE(D17:D19)</f>
-        <v>75</v>
-      </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>60</v>
@@ -6366,21 +5224,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AAE13A-BA79-4C72-AD71-9A7DE004BCEA}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6391,12 +5249,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <v>55</v>
@@ -6406,40 +5264,40 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H6" s="1">
         <f>AVERAGE(F4:F8)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>10</v>
@@ -6449,45 +5307,45 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>45</v>
@@ -6497,40 +5355,40 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H16" s="1">
         <f>AVERAGE(F14:F18)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <v>85</v>
@@ -6540,12 +5398,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>60</v>
@@ -6561,21 +5419,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721C6819-73FF-4AA8-8106-87D063E517F6}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1"/>
-    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6586,145 +5444,145 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H6" s="1">
         <f>AVERAGE(D4:D10)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H16" s="1">
         <f>AVERAGE(D13:D19)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>60</v>

</xml_diff>